<commit_message>
CSE474 OFFLINE3, half done
</commit_message>
<xml_diff>
--- a/CSE472/Offline3/Results_1305043.xlsx
+++ b/CSE472/Offline3/Results_1305043.xlsx
@@ -185,14 +185,14 @@
   <dimension ref="B1:F21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -242,16 +242,16 @@
         <v>10</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>2.10811320747748</v>
+        <v>0.819402704056875</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>2.10878957568109</v>
+        <v>0.775051439637763</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>2.10053907795764</v>
+        <v>0.801025969828675</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>2.0508678520409</v>
+        <v>0.928403411130697</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,16 +259,16 @@
         <v>20</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>2.13928763391418</v>
+        <v>0.562082010351434</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>2.14479486000829</v>
+        <v>0.552962097649074</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>2.12367629026464</v>
+        <v>0.585287783208194</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>2.0244128665313</v>
+        <v>0.854073613966128</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -276,16 +276,16 @@
         <v>40</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>2.85135436733145</v>
+        <v>0.222858457658676</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>2.45939751461086</v>
+        <v>0.211689990670374</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>2.20111016925957</v>
+        <v>0.298868873298056</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>1.97080187281477</v>
+        <v>0.874983841162522</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -335,16 +335,16 @@
         <v>10</v>
       </c>
       <c r="C12" s="5" t="n">
-        <v>1.24228549687558</v>
+        <v>0.958707283679204</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>1.37922272860414</v>
+        <v>0.960188377135612</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>1.27518373565971</v>
+        <v>0.949663040567693</v>
       </c>
       <c r="F12" s="5" t="n">
-        <v>1.23954273707981</v>
+        <v>0.983660028016208</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -352,16 +352,16 @@
         <v>20</v>
       </c>
       <c r="C13" s="5" t="n">
-        <v>1.39789064269054</v>
+        <v>0.865610485637818</v>
       </c>
       <c r="D13" s="5" t="n">
-        <v>1.34316954586207</v>
+        <v>0.867606451132059</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>1.4001585552044</v>
+        <v>0.87093870187506</v>
       </c>
       <c r="F13" s="5" t="n">
-        <v>1.1596646109315</v>
+        <v>0.95669128535637</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -369,16 +369,16 @@
         <v>40</v>
       </c>
       <c r="C14" s="5" t="n">
-        <v>2.9284783464108</v>
+        <v>0.705492603737855</v>
       </c>
       <c r="D14" s="5" t="n">
-        <v>2.06951298594737</v>
+        <v>0.694408799265067</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>1.57934419855095</v>
+        <v>0.702073984969587</v>
       </c>
       <c r="F14" s="5" t="n">
-        <v>1.0701911444648</v>
+        <v>0.945423353622081</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,28 +427,52 @@
       <c r="B19" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="C19" s="5" t="n">
+        <v>1.08157893901907</v>
+      </c>
+      <c r="D19" s="5" t="n">
+        <v>1.08538228022025</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>1.07293191044207</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <v>1.11604897913846</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="C20" s="5" t="n">
+        <v>0.962551200148463</v>
+      </c>
+      <c r="D20" s="5" t="n">
+        <v>0.964462006793618</v>
+      </c>
+      <c r="E20" s="5" t="n">
+        <v>0.97463378415388</v>
+      </c>
+      <c r="F20" s="5" t="n">
+        <v>1.08147900935051</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="C21" s="5" t="n">
+        <v>0.763065037439799</v>
+      </c>
+      <c r="D21" s="5" t="n">
+        <v>0.775224764725676</v>
+      </c>
+      <c r="E21" s="5" t="n">
+        <v>0.786992541953138</v>
+      </c>
+      <c r="F21" s="5" t="n">
+        <v>1.0698128993807</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>